<commit_message>
Global : Suppression du serveur intermédiaire pour le host des queues User stories : Ajout des user stories concernant l'architecture virtuelle
</commit_message>
<xml_diff>
--- a/User stories.xlsx
+++ b/User stories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
   <si>
     <t>Serveur WEB</t>
   </si>
@@ -232,6 +232,24 @@
   </si>
   <si>
     <t>Tâche n°9:</t>
+  </si>
+  <si>
+    <t>Maquette index.xhtml</t>
+  </si>
+  <si>
+    <t>Intégration index.xhtml</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Création de l'architecture vSphere</t>
+  </si>
+  <si>
+    <t>Création de la solution de stockage SAN</t>
+  </si>
+  <si>
+    <t>Haute disponibilité pour le seveur web et le serveur Core</t>
   </si>
 </sst>
 </file>
@@ -412,6 +430,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,19 +443,143 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="24">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -581,7 +727,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -590,6 +736,12 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -705,13 +857,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -724,6 +869,25 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -740,23 +904,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:F7" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:F7" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A2:F7"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="13"/>
-    <tableColumn id="2" name="Nom" dataDxfId="12"/>
-    <tableColumn id="3" name="Importance" dataDxfId="11"/>
-    <tableColumn id="4" name="Estimation" dataDxfId="10"/>
-    <tableColumn id="5" name="Démo" dataDxfId="9"/>
-    <tableColumn id="6" name="Notes" dataDxfId="8"/>
+    <tableColumn id="1" name="ID" dataDxfId="19"/>
+    <tableColumn id="2" name="Nom" dataDxfId="18"/>
+    <tableColumn id="3" name="Importance" dataDxfId="17"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="16"/>
+    <tableColumn id="5" name="Démo" dataDxfId="15"/>
+    <tableColumn id="6" name="Notes" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau18" displayName="Tableau18" ref="A54:E57" totalsRowShown="0">
-  <autoFilter ref="A54:E57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau17" displayName="Tableau17" ref="A52:E54" totalsRowShown="0">
+  <autoFilter ref="A52:E54"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Tâche n°7:"/>
+    <tableColumn id="2" name="Opération sur fichier vidéo"/>
+    <tableColumn id="3" name="Type composant"/>
+    <tableColumn id="4" name="Estimation"/>
+    <tableColumn id="5" name="Sprint1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau18" displayName="Tableau18" ref="A57:E60" totalsRowShown="0">
+  <autoFilter ref="A57:E60"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Tâche n°8:"/>
     <tableColumn id="2" name="Reception et envois des vidéos au serveur Web"/>
@@ -768,9 +946,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau19" displayName="Tableau19" ref="A60:E68" totalsRowShown="0">
-  <autoFilter ref="A60:E68"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau19" displayName="Tableau19" ref="A63:E73" totalsRowShown="0">
+  <autoFilter ref="A63:E73"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Tâche n°9:"/>
     <tableColumn id="2" name="Création de la charte graphique de la console web admin"/>
@@ -783,21 +961,36 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A10:F14" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A10:F14" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A10:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" name="Nom" dataDxfId="5"/>
-    <tableColumn id="3" name="Importance" dataDxfId="4"/>
-    <tableColumn id="4" name="Estimation" dataDxfId="3"/>
-    <tableColumn id="5" name="Démo" dataDxfId="2"/>
-    <tableColumn id="6" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" name="Nom" dataDxfId="11"/>
+    <tableColumn id="3" name="Importance" dataDxfId="10"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="9"/>
+    <tableColumn id="5" name="Démo" dataDxfId="8"/>
+    <tableColumn id="6" name="Notes" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau62" displayName="Tableau62" ref="A17:F20" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A17:F20"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" name="Nom" dataDxfId="4"/>
+    <tableColumn id="3" name="Importance" dataDxfId="3"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="2"/>
+    <tableColumn id="5" name="Démo" dataDxfId="1"/>
+    <tableColumn id="6" name="Notes" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A1:E7" totalsRowShown="0">
   <autoFilter ref="A1:E7"/>
   <tableColumns count="5">
@@ -811,7 +1004,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau12" displayName="Tableau12" ref="A10:E15" totalsRowShown="0">
   <autoFilter ref="A10:E15"/>
   <tableColumns count="5">
@@ -825,7 +1018,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau13" displayName="Tableau13" ref="A18:E21" totalsRowShown="0">
   <autoFilter ref="A18:E21"/>
   <tableColumns count="5">
@@ -839,7 +1032,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau14" displayName="Tableau14" ref="A24:E27" totalsRowShown="0">
   <autoFilter ref="A24:E27"/>
   <tableColumns count="5">
@@ -853,9 +1046,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau15" displayName="Tableau15" ref="A30:E38" totalsRowShown="0">
-  <autoFilter ref="A30:E38"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau15" displayName="Tableau15" ref="A30:E40" totalsRowShown="0">
+  <autoFilter ref="A30:E40"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Tâche n°5:"/>
     <tableColumn id="2" name="Création de la charte graphique du site"/>
@@ -867,26 +1060,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau16" displayName="Tableau16" ref="A41:E46" totalsRowShown="0">
-  <autoFilter ref="A41:E46"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau16" displayName="Tableau16" ref="A44:E49" totalsRowShown="0">
+  <autoFilter ref="A44:E49"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Tâche n°6:"/>
     <tableColumn id="2" name="Connection et configuration du server Core"/>
-    <tableColumn id="3" name="Type composant"/>
-    <tableColumn id="4" name="Estimation"/>
-    <tableColumn id="5" name="Sprint1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau17" displayName="Tableau17" ref="A49:E51" totalsRowShown="0">
-  <autoFilter ref="A49:E51"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Tâche n°7:"/>
-    <tableColumn id="2" name="Opération sur fichier vidéo"/>
     <tableColumn id="3" name="Type composant"/>
     <tableColumn id="4" name="Estimation"/>
     <tableColumn id="5" name="Sprint1"/>
@@ -1158,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,29 +1352,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1263,14 +1442,14 @@
       <c r="F7" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1340,25 +1519,93 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,7 +1658,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C5" t="s">
@@ -1509,7 +1756,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C19" t="s">
@@ -1624,222 +1871,248 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>55</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>12</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C44" t="s">
         <v>18</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D44" t="s">
         <v>4</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E44" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>60</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>62</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B52" t="s">
         <v>13</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C52" t="s">
         <v>18</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>4</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>63</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>64</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C54" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>65</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" t="s">
         <v>15</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C57" t="s">
         <v>18</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D57" t="s">
         <v>4</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>66</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>67</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>43</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C60" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>69</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>16</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C63" t="s">
         <v>18</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D63" t="s">
         <v>4</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E63" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>46</v>
-      </c>
-      <c r="C61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>47</v>
-      </c>
-      <c r="C62" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>48</v>
-      </c>
-      <c r="C63" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C64" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des tâches déjà réalisés pour les user stories: - Enregistrement et connexion utilisateurs - Connexion et configuration du serveur Core
</commit_message>
<xml_diff>
--- a/User stories.xlsx
+++ b/User stories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
   <si>
     <t>Serveur WEB</t>
   </si>
@@ -250,13 +250,16 @@
   </si>
   <si>
     <t>Haute disponibilité pour le seveur web et le serveur Core</t>
+  </si>
+  <si>
+    <t>Fait</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +270,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -420,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -446,6 +456,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -1339,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1604,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,6 +1651,9 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
+      <c r="D2" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1648,6 +1662,9 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
+      <c r="D3" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1656,6 +1673,9 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
+      <c r="D4" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
@@ -1664,6 +1684,7 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -1672,6 +1693,9 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="D6" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1680,6 +1704,9 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
+      <c r="D7" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1942,6 +1969,9 @@
       <c r="C47" t="s">
         <v>58</v>
       </c>
+      <c r="D47" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -1950,6 +1980,9 @@
       <c r="C48" t="s">
         <v>22</v>
       </c>
+      <c r="D48" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
@@ -1958,6 +1991,9 @@
       <c r="C49" t="s">
         <v>23</v>
       </c>
+      <c r="D49" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2117,8 +2153,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="9">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2127,6 +2163,7 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Signed-off-by: Tonyan7 <anthony.jonathan.laine@gmail.com> Global : Modification des paramètres de config (ajout nbWorker) User stories : Ajout des membres par tâche
</commit_message>
<xml_diff>
--- a/User stories.xlsx
+++ b/User stories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="81">
   <si>
     <t>Serveur WEB</t>
   </si>
@@ -253,6 +253,18 @@
   </si>
   <si>
     <t>Fait</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>Bastien</t>
+  </si>
+  <si>
+    <t>Omar et Dom</t>
   </si>
 </sst>
 </file>
@@ -444,6 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,13 +469,54 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -915,15 +969,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:F7" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:F7" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A2:F7"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="19"/>
-    <tableColumn id="2" name="Nom" dataDxfId="18"/>
-    <tableColumn id="3" name="Importance" dataDxfId="17"/>
-    <tableColumn id="4" name="Estimation" dataDxfId="16"/>
-    <tableColumn id="5" name="Démo" dataDxfId="15"/>
-    <tableColumn id="6" name="Notes" dataDxfId="14"/>
+    <tableColumn id="1" name="ID" dataDxfId="22"/>
+    <tableColumn id="2" name="Nom" dataDxfId="21"/>
+    <tableColumn id="3" name="Importance" dataDxfId="20"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="19"/>
+    <tableColumn id="5" name="Démo" dataDxfId="18"/>
+    <tableColumn id="6" name="Notes" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -936,7 +990,7 @@
     <tableColumn id="1" name="Tâche n°7:"/>
     <tableColumn id="2" name="Opération sur fichier vidéo"/>
     <tableColumn id="3" name="Type composant"/>
-    <tableColumn id="4" name="Estimation"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="0"/>
     <tableColumn id="5" name="Sprint1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -972,30 +1026,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A10:F14" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A10:F14" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A10:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="12"/>
-    <tableColumn id="2" name="Nom" dataDxfId="11"/>
-    <tableColumn id="3" name="Importance" dataDxfId="10"/>
-    <tableColumn id="4" name="Estimation" dataDxfId="9"/>
-    <tableColumn id="5" name="Démo" dataDxfId="8"/>
-    <tableColumn id="6" name="Notes" dataDxfId="7"/>
+    <tableColumn id="1" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" name="Nom" dataDxfId="14"/>
+    <tableColumn id="3" name="Importance" dataDxfId="13"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="12"/>
+    <tableColumn id="5" name="Démo" dataDxfId="11"/>
+    <tableColumn id="6" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau62" displayName="Tableau62" ref="A17:F20" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau62" displayName="Tableau62" ref="A17:F20" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A17:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" name="Nom" dataDxfId="4"/>
-    <tableColumn id="3" name="Importance" dataDxfId="3"/>
-    <tableColumn id="4" name="Estimation" dataDxfId="2"/>
-    <tableColumn id="5" name="Démo" dataDxfId="1"/>
-    <tableColumn id="6" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Nom" dataDxfId="7"/>
+    <tableColumn id="3" name="Importance" dataDxfId="6"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="5"/>
+    <tableColumn id="5" name="Démo" dataDxfId="4"/>
+    <tableColumn id="6" name="Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1022,7 +1076,7 @@
     <tableColumn id="1" name="Tâches n°2 :"/>
     <tableColumn id="2" name="Upload de fichier"/>
     <tableColumn id="3" name="Type composant"/>
-    <tableColumn id="4" name="Estimation"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="2"/>
     <tableColumn id="5" name="Sprint1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1078,7 +1132,7 @@
     <tableColumn id="1" name="Tâche n°6:"/>
     <tableColumn id="2" name="Connection et configuration du server Core"/>
     <tableColumn id="3" name="Type composant"/>
-    <tableColumn id="4" name="Estimation"/>
+    <tableColumn id="4" name="Estimation" dataDxfId="1"/>
     <tableColumn id="5" name="Sprint1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1351,7 +1405,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,14 +1417,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1453,14 +1507,14 @@
       <c r="F7" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1531,14 +1585,14 @@
       <c r="F14" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1616,7 +1670,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,7 +1705,10 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1662,7 +1719,10 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1673,7 +1733,10 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1684,7 +1747,9 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -1693,7 +1758,10 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1704,7 +1772,10 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1732,6 +1803,9 @@
       <c r="C11" t="s">
         <v>26</v>
       </c>
+      <c r="D11" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1740,6 +1814,9 @@
       <c r="C12" t="s">
         <v>19</v>
       </c>
+      <c r="D12" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1748,6 +1825,9 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
+      <c r="D13" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1756,6 +1836,9 @@
       <c r="C14" t="s">
         <v>41</v>
       </c>
+      <c r="D14" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1764,6 +1847,9 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
+      <c r="D15" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1830,6 +1916,9 @@
       <c r="C25" t="s">
         <v>41</v>
       </c>
+      <c r="D25" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -1838,6 +1927,9 @@
       <c r="C26" t="s">
         <v>42</v>
       </c>
+      <c r="D26" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -1846,6 +1938,9 @@
       <c r="C27" t="s">
         <v>44</v>
       </c>
+      <c r="D27" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1871,6 +1966,9 @@
       <c r="C31" t="s">
         <v>54</v>
       </c>
+      <c r="D31" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -1879,6 +1977,9 @@
       <c r="C32" t="s">
         <v>54</v>
       </c>
+      <c r="D32" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -1887,6 +1988,9 @@
       <c r="C33" t="s">
         <v>54</v>
       </c>
+      <c r="D33" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -1895,6 +1999,9 @@
       <c r="C34" t="s">
         <v>54</v>
       </c>
+      <c r="D34" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -1903,6 +2010,9 @@
       <c r="C35" t="s">
         <v>54</v>
       </c>
+      <c r="D35" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -1953,6 +2063,7 @@
       <c r="C45" t="s">
         <v>26</v>
       </c>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -1961,6 +2072,7 @@
       <c r="C46" t="s">
         <v>26</v>
       </c>
+      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -1969,7 +2081,8 @@
       <c r="C47" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="11"/>
+      <c r="E47" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1980,7 +2093,8 @@
       <c r="C48" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="11"/>
+      <c r="E48" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1991,7 +2105,8 @@
       <c r="C49" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="11"/>
+      <c r="E49" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2019,6 +2134,9 @@
       <c r="C53" t="s">
         <v>41</v>
       </c>
+      <c r="D53" s="11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
@@ -2026,6 +2144,9 @@
       </c>
       <c r="C54" t="s">
         <v>41</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>